<commit_message>
change delete logic (using 'ON DELETE CASCADE')
</commit_message>
<xml_diff>
--- a/doc/input.xlsx
+++ b/doc/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiida\github\builder\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9742950-8A51-4188-BAFC-3248DF8D5B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED6EA97-E6B2-45E9-89AB-5D35C4302B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="816" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6133,10 +6133,10 @@
   <dimension ref="A1:X181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -6945,6 +6945,9 @@
       <c r="N17" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="O17" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V17" s="7" t="s">
         <v>302</v>
       </c>
@@ -7616,6 +7619,9 @@
       <c r="N32" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="O32" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V32" s="7" t="s">
         <v>302</v>
       </c>
@@ -7996,6 +8002,9 @@
         <f>IF(ISBLANK(L41),"",VLOOKUP(L41,Field!$A:$D,3,FALSE)&amp;"."&amp;VLOOKUP(L41,Field!$A:$D,4,FALSE))</f>
         <v/>
       </c>
+      <c r="O41" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V41" s="7" t="s">
         <v>125</v>
       </c>
@@ -8035,6 +8044,9 @@
         <f>IF(ISBLANK(L42),"",VLOOKUP(L42,Field!$A:$D,3,FALSE)&amp;"."&amp;VLOOKUP(L42,Field!$A:$D,4,FALSE))</f>
         <v/>
       </c>
+      <c r="O42" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V42" s="7" t="s">
         <v>126</v>
       </c>
@@ -8073,6 +8085,9 @@
       <c r="M43" s="3" t="str">
         <f>IF(ISBLANK(L43),"",VLOOKUP(L43,Field!$A:$D,3,FALSE)&amp;"."&amp;VLOOKUP(L43,Field!$A:$D,4,FALSE))</f>
         <v/>
+      </c>
+      <c r="O43" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="V43" s="7" t="s">
         <v>127</v>
@@ -8608,6 +8623,9 @@
         <v/>
       </c>
       <c r="N57" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O57" s="3" t="b">
         <v>1</v>
       </c>
       <c r="V57" s="7" t="s">
@@ -9538,6 +9556,9 @@
       <c r="N79" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="O79" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V79" s="7" t="s">
         <v>302</v>
       </c>
@@ -10007,6 +10028,9 @@
         <v/>
       </c>
       <c r="N90" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O90" s="3" t="b">
         <v>1</v>
       </c>
       <c r="V90" s="7" t="s">
@@ -10412,6 +10436,9 @@
         <v/>
       </c>
       <c r="N99" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O99" s="3" t="b">
         <v>1</v>
       </c>
       <c r="V99" s="7" t="s">
@@ -12179,6 +12206,9 @@
         <f>IF(ISBLANK(L141),"",VLOOKUP(L141,Field!$A:$D,3,FALSE)&amp;"."&amp;VLOOKUP(L141,Field!$A:$D,4,FALSE))</f>
         <v/>
       </c>
+      <c r="O141" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="V141" s="6"/>
     </row>
     <row r="142" spans="1:24">
@@ -12778,7 +12808,9 @@
         <v/>
       </c>
       <c r="N155" s="6"/>
-      <c r="O155" s="6"/>
+      <c r="O155" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="P155" s="6"/>
       <c r="Q155" s="6"/>
       <c r="R155" s="6"/>

</xml_diff>

<commit_message>
Add id max value in summary.
</commit_message>
<xml_diff>
--- a/doc/input.xlsx
+++ b/doc/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiida\github\builder\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED395C9-5095-4C7B-95B7-6A5708B1F508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6278AAE6-5043-43C3-A07B-9105D343DCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="816" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="614">
   <si>
     <t>classId</t>
     <phoneticPr fontId="1"/>
@@ -4514,100 +4514,98 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C10E577-100B-4BAB-8A07-F8768560B049}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.6640625" style="3"/>
+    <col min="3" max="3" width="13.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
         <v>402</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>400</v>
+      <c r="C1" s="4" t="s">
+        <v>506</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>506</v>
+        <v>432</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>401</v>
+        <v>367</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>383</v>
+        <v>451</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="U1" s="4" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:20">
       <c r="A2" s="5">
         <f>ROW()-1</f>
         <v>1</v>
@@ -4619,21 +4617,21 @@
       <c r="C2" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>403</v>
+      </c>
       <c r="H2" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="I2" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>408</v>
+      </c>
       <c r="K2" s="5" t="s">
         <v>408</v>
       </c>
@@ -4644,27 +4642,24 @@
         <v>408</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q2" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="S2" s="5" t="s">
+        <v>406</v>
+      </c>
       <c r="T2" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="U2" s="5" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:20">
       <c r="A3" s="3">
         <f>ROW()-1</f>
         <v>2</v>
@@ -4676,21 +4671,18 @@
       <c r="C3" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <f>$A$2</f>
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <f>ROW()-1</f>
         <v>3</v>
@@ -4702,21 +4694,18 @@
       <c r="C4" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <f>$A$2</f>
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:20">
       <c r="A5" s="3">
         <f>ROW()-1</f>
         <v>4</v>
@@ -4728,21 +4717,18 @@
       <c r="C5" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <f>$A$2</f>
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:20">
       <c r="A6" s="3">
         <f>ROW()-1</f>
         <v>5</v>
@@ -4754,15 +4740,15 @@
       <c r="C6" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="6"/>
+      <c r="H6" s="3" t="s">
         <v>413</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>414</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>414</v>
@@ -4773,13 +4759,10 @@
       <c r="M6" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>414</v>
-      </c>
+      <c r="S6" s="6"/>
       <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-    </row>
-    <row r="7" spans="1:21">
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="3">
         <f t="shared" ref="A7" si="0">ROW()-1</f>
         <v>6</v>
@@ -4791,21 +4774,21 @@
       <c r="C7" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <f>$A$6</f>
         <v>5</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>446</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>447</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>447</v>
@@ -4817,15 +4800,12 @@
         <v>447</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="O7" s="3" t="s">
         <v>421</v>
       </c>
+      <c r="S7" s="6"/>
       <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="3">
         <f>ROW()-1</f>
         <v>7</v>
@@ -4837,14 +4817,14 @@
       <c r="C8" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>419</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>420</v>
@@ -4856,13 +4836,10 @@
         <v>420</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="O8" s="3" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:20">
       <c r="A9" s="3">
         <f>ROW()-1</f>
         <v>8</v>
@@ -4874,21 +4851,21 @@
       <c r="C9" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="3">
         <f>$A$8</f>
         <v>7</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>462</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="G9" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>423</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>438</v>
@@ -4899,11 +4876,8 @@
       <c r="M9" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="3">
         <f>ROW()-1</f>
         <v>9</v>
@@ -4915,21 +4889,18 @@
       <c r="C10" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="3">
         <f>A9</f>
         <v>8</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:20">
       <c r="A11" s="3">
         <f>ROW()-1</f>
         <v>10</v>
@@ -4939,19 +4910,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>448</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>457</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>448</v>
+      <c r="J11" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>438</v>
@@ -4960,9 +4931,6 @@
         <v>438</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="N11" s="3" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6584,10 +6552,10 @@
   <dimension ref="A1:X189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="K124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N136" sqref="N136"/>
+      <selection pane="bottomRight" activeCell="R160" sqref="R160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -6730,7 +6698,9 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+      <c r="R2" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -7551,7 +7521,9 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
+      <c r="R21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -8225,7 +8197,9 @@
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+      <c r="R36" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
@@ -9261,7 +9235,9 @@
       <c r="O62" s="8"/>
       <c r="P62" s="8"/>
       <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
+      <c r="R62" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S62" s="8"/>
       <c r="T62" s="8"/>
       <c r="U62" s="8"/>
@@ -9590,7 +9566,9 @@
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
+      <c r="R70" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5"/>
@@ -10628,7 +10606,9 @@
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
       <c r="Q94" s="5"/>
-      <c r="R94" s="5"/>
+      <c r="R94" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S94" s="5"/>
       <c r="T94" s="5"/>
       <c r="U94" s="5"/>
@@ -11002,7 +10982,9 @@
       <c r="O102" s="5"/>
       <c r="P102" s="5"/>
       <c r="Q102" s="5"/>
-      <c r="R102" s="5"/>
+      <c r="R102" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S102" s="5"/>
       <c r="T102" s="5"/>
       <c r="U102" s="5"/>
@@ -11877,7 +11859,9 @@
       <c r="O123" s="5"/>
       <c r="P123" s="5"/>
       <c r="Q123" s="5"/>
-      <c r="R123" s="5"/>
+      <c r="R123" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S123" s="5"/>
       <c r="T123" s="5"/>
       <c r="U123" s="5"/>
@@ -12045,7 +12029,9 @@
       <c r="O128" s="5"/>
       <c r="P128" s="5"/>
       <c r="Q128" s="5"/>
-      <c r="R128" s="5"/>
+      <c r="R128" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S128" s="5"/>
       <c r="T128" s="5"/>
       <c r="U128" s="5"/>
@@ -12253,7 +12239,9 @@
       <c r="O134" s="5"/>
       <c r="P134" s="5"/>
       <c r="Q134" s="5"/>
-      <c r="R134" s="5"/>
+      <c r="R134" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S134" s="5"/>
       <c r="T134" s="5"/>
       <c r="U134" s="5"/>
@@ -12467,7 +12455,9 @@
       <c r="O140" s="5"/>
       <c r="P140" s="5"/>
       <c r="Q140" s="5"/>
-      <c r="R140" s="5"/>
+      <c r="R140" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="S140" s="5"/>
       <c r="T140" s="5"/>
       <c r="U140" s="5"/>

</xml_diff>

<commit_message>
Add Layout json generating functions.
</commit_message>
<xml_diff>
--- a/doc/input.xlsx
+++ b/doc/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiida\github\builder\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B1C12-E9A5-4E4E-BBED-0CA7183E35B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692ACC04-AC2D-4476-AD2F-F750116FA99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="816" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="637">
   <si>
     <t>classId</t>
     <phoneticPr fontId="1"/>
@@ -3284,6 +3284,14 @@
     <rPh sb="9" eb="11">
       <t>ニュウシュツ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>root</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parent == null</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5633,7 +5641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7F7B46-C5DA-4B16-AA9F-5D00A52EB62D}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
@@ -6844,10 +6852,10 @@
   <dimension ref="A1:X187"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -17346,9 +17354,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9719863C-01F4-477F-A560-5CCC2301FB87}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -17500,6 +17510,21 @@
       </c>
       <c r="F7" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>Class!$A$18</f>
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>635</v>
+      </c>
+      <c r="D8" t="s">
+        <v>636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>